<commit_message>
primer commit en dev
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/Datos.xlsx
+++ b/src/test/resources/Data/Datos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\Testing\Alkomprar\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34078B7E-57B5-43D8-92A8-A86206B526B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140866C8-3279-4DED-A788-55CC25556264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31215" yWindow="2400" windowWidth="17250" windowHeight="8865" xr2:uid="{7B134272-501A-4985-B2FD-36C69D69ABC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>correo</t>
   </si>
@@ -50,64 +50,37 @@
     <t>telefono</t>
   </si>
   <si>
-    <t>prueba1@gmail.com</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Gutierrez</t>
-  </si>
-  <si>
     <t>3111111111</t>
   </si>
   <si>
     <t>3111111112</t>
   </si>
   <si>
-    <t>3111111113</t>
-  </si>
-  <si>
-    <t>3111111114</t>
-  </si>
-  <si>
-    <t>3111111115</t>
-  </si>
-  <si>
-    <t>prueba2@gmail.com</t>
-  </si>
-  <si>
-    <t>prueba3@gmail.com</t>
-  </si>
-  <si>
-    <t>prueba4@gmail.com</t>
-  </si>
-  <si>
-    <t>prueba5@gmail.com</t>
-  </si>
-  <si>
     <t>Jhon</t>
   </si>
   <si>
     <t>Pedro</t>
   </si>
   <si>
-    <t>Hernesto</t>
-  </si>
-  <si>
-    <t>Andres</t>
-  </si>
-  <si>
     <t>Gonzales</t>
   </si>
   <si>
     <t>Torres</t>
   </si>
   <si>
-    <t>Ardila</t>
-  </si>
-  <si>
-    <t>Perez</t>
+    <t>prueba2asg@gmail.com</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>pruebafinal6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -486,21 +459,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1043D73-F22C-4250-A2F2-0B19E05AFB8B}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -513,88 +487,54 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="4" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{F2EF09F6-44A3-4ADE-9C64-F542F579B1DE}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5F1EEBE0-0FEA-48E3-85D4-51937E45F35B}"/>
-    <hyperlink ref="A4:A6" r:id="rId3" display="prueba2@gmail.com" xr:uid="{D4EFA6E9-D9CE-4294-9297-8BDC4821C32A}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{5030E5BC-785E-4D07-B18D-C1AF5F3A0BDD}"/>
-    <hyperlink ref="A5" r:id="rId5" xr:uid="{4328B952-36E2-4C0C-9AEC-2889651D71F5}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{6D6684C5-E03D-4AF6-9BF5-0356F5234E66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>